<commit_message>
manual exported emg data added
</commit_message>
<xml_diff>
--- a/tutorials/repeated_sprinting/Simulations/EMG signals (quality control).xlsx
+++ b/tutorials/repeated_sprinting/Simulations/EMG signals (quality control).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e0adc246493e65f/Радна површина/Thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\opensim_tutorial\tutorials\repeated_sprinting\Simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="388" documentId="8_{B3162CB8-B385-45D3-B8EE-F5B8C58EBC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F010EBF5-7555-46B0-A247-8857F675E9DF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE1D12B-9559-46D0-A373-09B6B762DC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3084" yWindow="3816" windowWidth="17280" windowHeight="9960" xr2:uid="{BB286027-6DB6-4CA3-898C-4B0E1DE6441F}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" firstSheet="3" activeTab="6" xr2:uid="{BB286027-6DB6-4CA3-898C-4B0E1DE6441F}"/>
   </bookViews>
   <sheets>
     <sheet name="PC002" sheetId="1" r:id="rId1"/>
@@ -194,10 +194,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B252A99-EBBC-4C82-BBE6-041FB046FECD}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,7 +585,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -633,7 +633,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1118,7 +1118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CE3BD3-7389-4416-AF7F-CC98B0E70830}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1642,7 +1642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E727EEF3-8C8D-4DEC-A16A-3E714D63676A}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>

</xml_diff>